<commit_message>
lite some code and update the databas
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kazaf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\Kazaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="25515" windowHeight="15540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jan" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="137">
   <si>
     <t>日期</t>
     <rPh sb="0" eb="1">
@@ -1256,13 +1256,185 @@
     <rPh sb="7" eb="8">
       <t>yue hui</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桂斌结婚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>万象城买水和卫生纸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上跟赵总孙婧恩唱歌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买了件niketee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上百丽吃的赛百味</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百丽买的可乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给妈妈充话费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百丽广场买的水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请陈昊孚喝的星巴克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请大鹏吃的春川铁板鸡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中午吃的麦当劳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上沐青汤泉搓背</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给车子加油</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当当网上买的书《Spring Boot》，《Linux》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amazon买的打底衫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟吕文凯晚上打的实况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停车买水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给小弟红包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上踢球买水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭赛百味</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>踢球费用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中午请王艳明和孙校碰吃的小灶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上自己吃的润拉面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上买的西瓜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中午自己去百丽吃的赛百味</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车子加油</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请爸爸姥姥吃的面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上去跟哥哥们吃饭路费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上买的蓝牙键盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午买的面包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中午去良子足疗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上去火车站接妈妈买的玉米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百丽超市买水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uniqlo买的衣服</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭吃的港太兴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上海信大厦喝的东西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车子保养</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看球房间费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看球赛零食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百丽买的燕麦和果汁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买的牛奶和卫生纸</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1312,6 +1484,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1584,7 +1759,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1597,7 +1772,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1610,7 +1785,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,7 +1798,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1636,7 +1811,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1651,9 +1826,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -2282,11 +2457,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -3024,12 +3199,631 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>800</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5">
+        <v>144</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>42493</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>42493</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>2.7</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>42493</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>42496</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>42496</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>42497</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11">
+        <v>320</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>42498</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>42498</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>99</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>42498</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>42500</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15">
+        <v>159.9</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>42501</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16">
+        <v>470</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>42504</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>42504</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>11.5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>42505</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>42507</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>42507</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
+        <v>42507</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
+        <v>42507</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
+        <v>42510</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24">
+        <v>229</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
+        <v>42510</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
+        <v>42511</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
+        <v>42511</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="1">
+        <v>42512</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28">
+        <v>306</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
+        <v>42512</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
+        <v>42512</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
+        <v>42512</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31">
+        <v>382.79</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
+        <v>42513</v>
+      </c>
+      <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32">
+        <v>4.84</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
+        <v>42514</v>
+      </c>
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33">
+        <v>76</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
+        <v>42514</v>
+      </c>
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
+        <v>42517</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
+        <v>42517</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36">
+        <v>39</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
+        <v>42517</v>
+      </c>
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37">
+        <v>173</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
+        <v>42517</v>
+      </c>
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
+        <v>42518</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39">
+        <v>450</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
+        <v>42518</v>
+      </c>
+      <c r="B40" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
+        <v>42518</v>
+      </c>
+      <c r="B41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41">
+        <v>166</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
+        <v>42518</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42">
+        <v>93.5</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
+        <v>42519</v>
+      </c>
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43">
+        <v>23.8</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
+        <v>42520</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3041,7 +3835,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3054,7 +3848,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3067,7 +3861,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3080,7 +3874,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>